<commit_message>
Fix sprites for new nations.
</commit_message>
<xml_diff>
--- a/BaseI.xlsx
+++ b/BaseI.xlsx
@@ -16,15 +16,15 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="BaseI" localSheetId="0">Sheet1!$A$1:$FC$380</definedName>
-    <definedName name="BaseI_1" localSheetId="0">Sheet1!$A$1:$FC$380</definedName>
+    <definedName name="BaseI" localSheetId="0">Sheet1!$A$1:$FG$380</definedName>
+    <definedName name="BaseI_1" localSheetId="0">Sheet1!$A$1:$FG$380</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="941" uniqueCount="552">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="556">
   <si>
     <t>id</t>
   </si>
@@ -1680,6 +1680,18 @@
   </si>
   <si>
     <t>patience</t>
+  </si>
+  <si>
+    <t>retinue</t>
+  </si>
+  <si>
+    <t>restricted4</t>
+  </si>
+  <si>
+    <t>restricted5</t>
+  </si>
+  <si>
+    <t>restricted6</t>
   </si>
 </sst>
 </file>
@@ -1997,11 +2009,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AMO431"/>
+  <dimension ref="A1:AMS431"/>
   <sheetViews>
     <sheetView windowProtection="1" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2:FC400"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2138,14 +2150,17 @@
     <col min="139" max="139" width="12.81640625" collapsed="1"/>
     <col min="140" max="140" width="35.81640625" collapsed="1"/>
     <col min="141" max="141" width="81.1796875" collapsed="1"/>
-    <col min="142" max="154" width="15.453125" collapsed="1"/>
-    <col min="157" max="157" width="14.453125" bestFit="1" customWidth="1"/>
-    <col min="158" max="158" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="159" max="159" width="4.453125" collapsed="1"/>
-    <col min="160" max="1029" width="8.54296875" collapsed="1"/>
+    <col min="142" max="145" width="15.453125" collapsed="1"/>
+    <col min="146" max="148" width="9.7265625" bestFit="1" customWidth="1"/>
+    <col min="149" max="157" width="15.453125" collapsed="1"/>
+    <col min="160" max="160" width="14.453125" bestFit="1" customWidth="1"/>
+    <col min="161" max="161" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="162" max="162" width="8.7265625" customWidth="1"/>
+    <col min="163" max="163" width="4.453125" collapsed="1"/>
+    <col min="164" max="1033" width="8.54296875" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:163" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2582,49 +2597,61 @@
         <v>142</v>
       </c>
       <c r="EP1" t="s">
+        <v>553</v>
+      </c>
+      <c r="EQ1" t="s">
+        <v>554</v>
+      </c>
+      <c r="ER1" t="s">
+        <v>555</v>
+      </c>
+      <c r="ES1" t="s">
         <v>143</v>
       </c>
-      <c r="EQ1" t="s">
+      <c r="ET1" t="s">
         <v>144</v>
       </c>
-      <c r="ER1" t="s">
+      <c r="EU1" t="s">
         <v>145</v>
       </c>
-      <c r="ES1" t="s">
+      <c r="EV1" t="s">
         <v>146</v>
       </c>
-      <c r="ET1" t="s">
+      <c r="EW1" t="s">
         <v>147</v>
       </c>
-      <c r="EU1" t="s">
+      <c r="EX1" t="s">
         <v>148</v>
       </c>
-      <c r="EV1" t="s">
+      <c r="EY1" t="s">
         <v>149</v>
       </c>
-      <c r="EW1" t="s">
+      <c r="EZ1" t="s">
         <v>150</v>
       </c>
-      <c r="EX1" t="s">
+      <c r="FA1" t="s">
         <v>151</v>
       </c>
-      <c r="EY1" t="s">
+      <c r="FB1" t="s">
         <v>542</v>
       </c>
-      <c r="EZ1" t="s">
+      <c r="FC1" t="s">
         <v>543</v>
       </c>
-      <c r="FA1" t="s">
+      <c r="FD1" t="s">
         <v>550</v>
       </c>
-      <c r="FB1" t="s">
+      <c r="FE1" t="s">
         <v>551</v>
       </c>
-      <c r="FC1" t="s">
+      <c r="FF1" t="s">
+        <v>552</v>
+      </c>
+      <c r="FG1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="2" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:163" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2635,7 +2662,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="3" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:163" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2646,7 +2673,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="4" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:163" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2657,7 +2684,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="5" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:163" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2668,7 +2695,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="6" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:163" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2679,7 +2706,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="7" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:163" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2690,7 +2717,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="8" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:163" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2701,7 +2728,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="9" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:163" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2712,7 +2739,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="10" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:163" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2723,7 +2750,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="11" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:163" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2734,7 +2761,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="12" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:163" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2745,7 +2772,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="13" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:163" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2756,7 +2783,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="14" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:163" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2767,7 +2794,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="15" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:163" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2778,7 +2805,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="16" spans="1:159" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:163" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>

</xml_diff>